<commit_message>
update: major change: sync db & template update
</commit_message>
<xml_diff>
--- a/server/templates/template.xlsx
+++ b/server/templates/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12300" tabRatio="789" activeTab="1"/>
+    <workbookView windowWidth="27945" windowHeight="12300" tabRatio="789" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="スタート" sheetId="9" r:id="rId1"/>
@@ -6790,7 +6790,7 @@
                   <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76e3fe18-ad05-4723-99b8-eef611d0ac94}" type="VALUE">
+                    <a:fld id="{9138d217-891e-49d2-8955-9ee2cf0b1ccd}" type="VALUE">
                       <a:t>[VALUE]</a:t>
                     </a:fld>
                     <a:endParaRPr b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -7678,7 +7678,7 @@
                   <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{f3aa77c1-f829-4874-a584-6f000c39f311}" type="VALUE">
+                    <a:fld id="{98201cbc-3766-4904-bea4-2ff80263918f}" type="VALUE">
                       <a:t>[VALUE]</a:t>
                     </a:fld>
                     <a:endParaRPr b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -9730,7 +9730,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>169334</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1676400" cy="580676"/>
+    <xdr:ext cx="1676400" cy="590201"/>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -9739,7 +9739,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2643505" y="2698750"/>
-          <a:ext cx="1676400" cy="581025"/>
+          <a:ext cx="1676400" cy="590550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9787,7 +9787,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>186267</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1964267" cy="580676"/>
+    <xdr:ext cx="1964267" cy="590201"/>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -9796,7 +9796,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4277360" y="2715895"/>
-          <a:ext cx="1964055" cy="580390"/>
+          <a:ext cx="1964055" cy="589915"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9852,7 +9852,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4286250" y="3834130"/>
+          <a:off x="4286250" y="3843655"/>
           <a:ext cx="1625600" cy="607695"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9978,7 +9978,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7211695" y="2720340"/>
+          <a:off x="7211695" y="2729865"/>
           <a:ext cx="2962910" cy="467995"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10120,7 +10120,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10212070" y="2720340"/>
+          <a:off x="10212070" y="2729865"/>
           <a:ext cx="558800" cy="467995"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10312,7 +10312,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="268605" y="2720340"/>
+          <a:off x="268605" y="2729865"/>
           <a:ext cx="462915" cy="485140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10393,7 +10393,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10720070" y="7004050"/>
+          <a:off x="10720070" y="7013575"/>
           <a:ext cx="1859280" cy="626110"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -13916,8 +13916,8 @@
   </sheetPr>
   <dimension ref="B1:R65"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="90" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -15421,7 +15421,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="112">
-        <f>④経費!F12</f>
+        <f>④経費!F4</f>
         <v>0</v>
       </c>
       <c r="H41" s="113"/>
@@ -15459,7 +15459,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="115">
-        <f>④経費!F13</f>
+        <f>④経費!F5</f>
         <v>0</v>
       </c>
       <c r="H42" s="81"/>
@@ -15497,6 +15497,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="115">
+        <f>④経費!F6</f>
         <v>0</v>
       </c>
       <c r="H43" s="81"/>
@@ -15534,7 +15535,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="115">
-        <f>④経費!F15</f>
+        <f>④経費!F7</f>
         <v>0</v>
       </c>
       <c r="H44" s="78"/>
@@ -15574,7 +15575,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="115">
-        <f>④経費!F16</f>
+        <f>④経費!F8</f>
         <v>0</v>
       </c>
       <c r="H45" s="104"/>
@@ -15605,7 +15606,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="115">
-        <f>④経費!F17</f>
+        <f>④経費!F9</f>
         <v>0</v>
       </c>
       <c r="H46" s="78"/>
@@ -15638,7 +15639,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="115">
-        <f>④経費!F18</f>
+        <f>④経費!F10</f>
         <v>0</v>
       </c>
       <c r="H47" s="81"/>
@@ -15660,7 +15661,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="115">
-        <f>④経費!F19</f>
+        <f>④経費!F11</f>
         <v>0</v>
       </c>
       <c r="H48" s="81"/>
@@ -15682,7 +15683,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="115">
-        <f>④経費!F20</f>
+        <f>④経費!F12</f>
         <v>0</v>
       </c>
       <c r="H49" s="81"/>
@@ -21890,7 +21891,7 @@
   </sheetPr>
   <dimension ref="B1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:E12"/>
     </sheetView>
   </sheetViews>
@@ -22099,7 +22100,7 @@
       <c r="S11" s="458"/>
       <c r="T11" s="459"/>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" ht="15.75" spans="2:20">
       <c r="B12" s="431"/>
       <c r="C12" s="432"/>
       <c r="D12" s="432"/>
@@ -24142,7 +24143,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:L2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>